<commit_message>
jh forms renamed (template folder & thread_export_schoolforms);search = gradeLevel>10
</commit_message>
<xml_diff>
--- a/Project Files/Forms System (SHS)/exports/jh_sf8.xlsx
+++ b/Project Files/Forms System (SHS)/exports/jh_sf8.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2294" uniqueCount="91">
   <si>
     <t>Department of Education</t>
   </si>
@@ -234,55 +234,130 @@
     <t>Crossing Bayabas National High School</t>
   </si>
   <si>
-    <t>2019-2020</t>
-  </si>
-  <si>
-    <t>Grade 7</t>
-  </si>
-  <si>
-    <t>FIDELITY</t>
+    <t>2021-2022</t>
+  </si>
+  <si>
+    <t>Grade 12</t>
+  </si>
+  <si>
+    <t>SUNFLOWER</t>
   </si>
   <si>
     <t>Toril</t>
   </si>
   <si>
-    <t>01/29/2020</t>
+    <t>09/29/2021</t>
   </si>
   <si>
     <t>Male</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>903748234568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charlton, Mark </t>
+  </si>
+  <si>
+    <t>10/16/2004</t>
+  </si>
+  <si>
+    <t>16: 11</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>2.5600</t>
+  </si>
+  <si>
+    <t>16.4</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>903748834565</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hil, Ren </t>
+  </si>
+  <si>
+    <t>17: 0</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>22500.0000</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>234567880123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan, Romeo </t>
+  </si>
+  <si>
+    <t>Unmeasured</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>346772145678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jay, Clark </t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>903748234565</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joey, Yeoj </t>
+  </si>
+  <si>
     <t>Female</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>123543457474</t>
-  </si>
-  <si>
-    <t>Paderogao, Phil Rey, E. Jr</t>
-  </si>
-  <si>
-    <t>12/11/2006</t>
-  </si>
-  <si>
-    <t>15: 10</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>2.2500</t>
-  </si>
-  <si>
-    <t>17.7</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>345072145678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charmel, Jance </t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>17.5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>345672145678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jai, Jenicel </t>
   </si>
 </sst>
 </file>
@@ -1888,157 +1963,197 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="21" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
       <c r="G12" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="21"/>
+        <v>58</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="I12" s="21" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
+        <v>61</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="O12" s="21"/>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="21" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
       <c r="F13" s="34"/>
       <c r="G13" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="L13" s="21" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O13" s="21"/>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="21" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
       <c r="F14" s="34"/>
       <c r="G14" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="21"/>
+        <v>58</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>75</v>
+      </c>
       <c r="I14" s="21" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
+        <v>71</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="L14" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>75</v>
+      </c>
       <c r="O14" s="21"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="21" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
       <c r="F15" s="34"/>
       <c r="G15" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="21"/>
+        <v>58</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>75</v>
+      </c>
       <c r="I15" s="21" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
+        <v>71</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="L15" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="M15" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="N15" s="21" t="s">
+        <v>75</v>
+      </c>
       <c r="O15" s="21"/>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="21" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
       <c r="F16" s="34"/>
       <c r="G16" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="21"/>
+        <v>58</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="I16" s="21" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
+        <v>69</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>25</v>
+      </c>
       <c r="O16" s="21"/>
     </row>
     <row r="17" spans="1:15">
@@ -2046,7 +2161,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="C17" s="34" t="s">
         <v>32</v>
@@ -2072,60 +2187,80 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="21" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
       <c r="F18" s="34"/>
       <c r="G18" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" s="21"/>
+        <v>58</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="I18" s="21" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="J18" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
+        <v>61</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M18" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N18" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="O18" s="21"/>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="21" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
       <c r="F19" s="34"/>
       <c r="G19" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H19" s="21"/>
+        <v>58</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>75</v>
+      </c>
       <c r="I19" s="21" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="J19" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
+        <v>71</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="L19" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="N19" s="21" t="s">
+        <v>75</v>
+      </c>
       <c r="O19" s="21"/>
     </row>
     <row r="20" spans="1:15">
@@ -2360,38 +2495,38 @@
       </c>
       <c r="B28" s="36"/>
       <c r="C28" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" s="50"/>
       <c r="E28" s="9" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N28" s="50" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="O28" s="50"/>
     </row>
@@ -2401,38 +2536,38 @@
       </c>
       <c r="B29" s="37"/>
       <c r="C29" s="56" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D29" s="56"/>
       <c r="E29" s="11" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="K29" s="11" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="L29" s="11" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="N29" s="56" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="O29" s="56"/>
     </row>
@@ -2442,38 +2577,38 @@
       </c>
       <c r="B30" s="38"/>
       <c r="C30" s="57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="13" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M30" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N30" s="57" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="O30" s="57"/>
     </row>

</xml_diff>